<commit_message>
feat: Sistema de listas de precios por jerarquía con autenticación por roles
- Agregar tablas ListasPrecios y PreciosCalculados con rangos por nivel
- Implementar 3 niveles de jerarquía:
  * Vendedor: 90% a 65% sobre Mark-up
  * Gerencia Comercial: 65% a 40% sobre Mark-up
  * Gerencia: 40% a 10% sobre Mark-up
- Calcular 854 listas de precios (427 SKUs  2 transportes)
- Crear endpoint /auth/me para obtener información del usuario
- Implementar vistas personalizadas por rol en frontend
- Admin y Gerencia ven costos completos (Costo Base, Flete%, Seguro%, Arancel%, DTA%, Hon.Aduanales%, Landed Cost, Mark-up)
- Vendedores solo ven sus rangos de precios autorizados
- Agregar función calculate_price_lists() en cost_engine.py
- Actualizar schemas con ListaPrecio incluyendo campos de costos
- Modificar frontend para renderizar tablas dinámicas según rol
- Descarga Excel filtrada por rol con información autorizada
- 4 usuarios de prueba: admin, gerencia1, gercom1, vendedor1
</commit_message>
<xml_diff>
--- a/Plantilla_Pricing_Costos_Importacion.xlsx
+++ b/Plantilla_Pricing_Costos_Importacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FernandoOlveraRendon\Documents\Base_Costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BFE384-098B-443F-9602-C11EE143CDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5379E5D1-40CD-4F01-B7B2-8E26B3C6267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3917" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3919" uniqueCount="902">
   <si>
     <t>SKU</t>
   </si>
@@ -3007,7 +3007,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblCatalogo" displayName="tblCatalogo" ref="A1:K428" headerRowCellStyle="Normal" dataCellStyle="Normal" totalsRowCellStyle="Normal">
-  <autoFilter ref="A1:K428" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K197">
     <sortCondition sortBy="fontColor" ref="A1:A197" dxfId="4"/>
   </sortState>
@@ -3346,7 +3345,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18677,7 +18676,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18739,7 +18738,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>813</v>
+        <v>469</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>162</v>
@@ -18754,7 +18753,7 @@
       </c>
       <c r="E2" s="2">
         <f>_xlfn.XLOOKUP(A2,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
-        <v>35</v>
+        <v>3000</v>
       </c>
       <c r="F2" s="2">
         <f>_xlfn.XLOOKUP(D2,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
@@ -18762,7 +18761,7 @@
       </c>
       <c r="G2" s="7">
         <f>$E2*$F2</f>
-        <v>735</v>
+        <v>63000</v>
       </c>
       <c r="H2" s="8">
         <f>_xlfn.XLOOKUP($B$2,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -18790,24 +18789,72 @@
       </c>
       <c r="N2" s="2">
         <f>IF($C2="Importado",$G2*(1+$H2+I2+$J2+$L2+$M2),$G2)</f>
-        <v>1005.8475000000001</v>
+        <v>86215.5</v>
       </c>
       <c r="O2" s="2">
         <f>N2 * (1 + K2)</f>
-        <v>1106.4322500000001</v>
+        <v>94837.05</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="A3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xlfn.XLOOKUP(A3,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!F:F,"",0)</f>
+        <v>Importado</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xlfn.XLOOKUP(A3,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!I:I,"",0)</f>
+        <v>USD</v>
+      </c>
+      <c r="E3" s="2">
+        <f>_xlfn.XLOOKUP(A3,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
+        <v>3000</v>
+      </c>
+      <c r="F3" s="2">
+        <f>_xlfn.XLOOKUP(D3,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
+        <v>21</v>
+      </c>
+      <c r="G3" s="7">
+        <f>$E3*$F3</f>
+        <v>63000</v>
+      </c>
+      <c r="H3" s="8">
+        <f>_xlfn.XLOOKUP($B$3,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>1.2</v>
+      </c>
+      <c r="I3" s="8">
+        <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J3" s="8">
+        <f>_xlfn.XLOOKUP("Arancel",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.05</v>
+      </c>
+      <c r="K3" s="8">
+        <f>_xlfn.XLOOKUP("Mark_up",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="8">
+        <f>_xlfn.XLOOKUP("DTA",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="M3" s="11">
+        <f>_xlfn.XLOOKUP("Honorarios_Aduanales",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="N3" s="2">
+        <f>IF($C3="Importado",$G3*(1+$H3+I3+$J3+$L3+$M3),$G3)</f>
+        <v>142915.5</v>
+      </c>
+      <c r="O3" s="2">
+        <f>N3 * (1 + K3)</f>
+        <v>157207.05000000002</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E4" s="2"/>
@@ -42783,7 +42830,7 @@
           <x14:formula1>
             <xm:f>PARAMETROS_IMPORTACION!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
+          <xm:sqref>B2:B3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fix: Gerencia_Comercial ahora ve todas las columnas de costos. Actualiza jerarquía completa con 5 niveles y contraseñas estandarizadas
</commit_message>
<xml_diff>
--- a/Plantilla_Pricing_Costos_Importacion.xlsx
+++ b/Plantilla_Pricing_Costos_Importacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FernandoOlveraRendon\Documents\Base_Costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5379E5D1-40CD-4F01-B7B2-8E26B3C6267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E50388-3494-41B0-A6F0-C2CC8D2071CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CATALOGO_PRODUCTOS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3919" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3920" uniqueCount="903">
   <si>
     <t>SKU</t>
   </si>
@@ -2803,6 +2803,9 @@
   </si>
   <si>
     <t>Honorarios_Aduanales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipo  10 aereo y 5 maritimo </t>
   </si>
 </sst>
 </file>
@@ -3343,9 +3346,9 @@
   </sheetPr>
   <dimension ref="A1:L428"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3893,6 +3896,9 @@
       </c>
       <c r="K15" t="s">
         <v>77</v>
+      </c>
+      <c r="L15" t="s">
+        <v>902</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -18674,9 +18680,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18738,7 +18744,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>469</v>
+        <v>79</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>162</v>
@@ -18753,7 +18759,7 @@
       </c>
       <c r="E2" s="2">
         <f>_xlfn.XLOOKUP(A2,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
-        <v>3000</v>
+        <v>415</v>
       </c>
       <c r="F2" s="2">
         <f>_xlfn.XLOOKUP(D2,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
@@ -18761,7 +18767,7 @@
       </c>
       <c r="G2" s="7">
         <f>$E2*$F2</f>
-        <v>63000</v>
+        <v>8715</v>
       </c>
       <c r="H2" s="8">
         <f>_xlfn.XLOOKUP($B$2,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -18789,16 +18795,16 @@
       </c>
       <c r="N2" s="2">
         <f>IF($C2="Importado",$G2*(1+$H2+I2+$J2+$L2+$M2),$G2)</f>
-        <v>86215.5</v>
+        <v>11926.477500000001</v>
       </c>
       <c r="O2" s="2">
         <f>N2 * (1 + K2)</f>
-        <v>94837.05</v>
+        <v>13119.125250000003</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>469</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>166</v>
@@ -18813,7 +18819,7 @@
       </c>
       <c r="E3" s="2">
         <f>_xlfn.XLOOKUP(A3,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
-        <v>3000</v>
+        <v>415</v>
       </c>
       <c r="F3" s="2">
         <f>_xlfn.XLOOKUP(D3,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
@@ -18821,7 +18827,7 @@
       </c>
       <c r="G3" s="7">
         <f>$E3*$F3</f>
-        <v>63000</v>
+        <v>8715</v>
       </c>
       <c r="H3" s="8">
         <f>_xlfn.XLOOKUP($B$3,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -18849,11 +18855,11 @@
       </c>
       <c r="N3" s="2">
         <f>IF($C3="Importado",$G3*(1+$H3+I3+$J3+$L3+$M3),$G3)</f>
-        <v>142915.5</v>
+        <v>19769.977500000001</v>
       </c>
       <c r="O3" s="2">
         <f>N3 * (1 + K3)</f>
-        <v>157207.05000000002</v>
+        <v>21746.975250000003</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Productionization: logging, monitoreo, scripts, seguridad, optimización BD, frontend timeout, deployment docs
</commit_message>
<xml_diff>
--- a/Plantilla_Pricing_Costos_Importacion.xlsx
+++ b/Plantilla_Pricing_Costos_Importacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FernandoOlveraRendon\Documents\Base_Costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E50388-3494-41B0-A6F0-C2CC8D2071CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3E88BF-1274-4699-8A1D-390AA3E1B337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CATALOGO_PRODUCTOS" sheetId="1" r:id="rId1"/>
@@ -3346,7 +3346,7 @@
   </sheetPr>
   <dimension ref="A1:L428"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
     </sheetView>
@@ -18387,7 +18387,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18424,7 +18424,7 @@
         <v>163</v>
       </c>
       <c r="C2">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="D2" t="s">
         <v>164</v>
@@ -18441,7 +18441,7 @@
         <v>163</v>
       </c>
       <c r="C3">
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
       <c r="D3" t="s">
         <v>167</v>
@@ -18680,9 +18680,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O2000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18771,7 +18771,7 @@
       </c>
       <c r="H2" s="8">
         <f>_xlfn.XLOOKUP($B$2,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="I2" s="8">
         <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -18795,11 +18795,11 @@
       </c>
       <c r="N2" s="2">
         <f>IF($C2="Importado",$G2*(1+$H2+I2+$J2+$L2+$M2),$G2)</f>
-        <v>11926.477500000001</v>
+        <v>9747.7275000000009</v>
       </c>
       <c r="O2" s="2">
         <f>N2 * (1 + K2)</f>
-        <v>13119.125250000003</v>
+        <v>10722.500250000001</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -18831,7 +18831,7 @@
       </c>
       <c r="H3" s="8">
         <f>_xlfn.XLOOKUP($B$3,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
       <c r="I3" s="8">
         <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -18855,11 +18855,11 @@
       </c>
       <c r="N3" s="2">
         <f>IF($C3="Importado",$G3*(1+$H3+I3+$J3+$L3+$M3),$G3)</f>
-        <v>19769.977500000001</v>
+        <v>10183.477500000001</v>
       </c>
       <c r="O3" s="2">
         <f>N3 * (1 + K3)</f>
-        <v>21746.975250000003</v>
+        <v>11201.825250000002</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fix: normalización de roles, logs y manejo de comentarios en autorizaciones. Corrige errores de aprobación/rechazo y asegura consistencia en endpoints.
</commit_message>
<xml_diff>
--- a/Plantilla_Pricing_Costos_Importacion.xlsx
+++ b/Plantilla_Pricing_Costos_Importacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FernandoOlveraRendon\Documents\Base_Costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3E88BF-1274-4699-8A1D-390AA3E1B337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800D2B31-CE70-42CF-B85F-4A9A3FC29E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CATALOGO_PRODUCTOS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3920" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3921" uniqueCount="904">
   <si>
     <t>SKU</t>
   </si>
@@ -2806,6 +2806,9 @@
   </si>
   <si>
     <t xml:space="preserve">Equipo  10 aereo y 5 maritimo </t>
+  </si>
+  <si>
+    <t>todos los casetes descontar 50%</t>
   </si>
 </sst>
 </file>
@@ -3344,11 +3347,11 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:L428"/>
+  <dimension ref="A1:L429"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10096,7 +10099,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>129</v>
       </c>
@@ -10131,7 +10134,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>68</v>
       </c>
@@ -10166,7 +10169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>64</v>
       </c>
@@ -10201,7 +10204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>150</v>
       </c>
@@ -10236,7 +10239,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>153</v>
       </c>
@@ -10271,7 +10274,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>485</v>
       </c>
@@ -10306,7 +10309,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>488</v>
       </c>
@@ -10340,8 +10343,11 @@
       <c r="K199" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L199">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>491</v>
       </c>
@@ -10375,8 +10381,11 @@
       <c r="K200" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L200">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>493</v>
       </c>
@@ -10410,8 +10419,11 @@
       <c r="K201" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L201">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>495</v>
       </c>
@@ -10445,8 +10457,11 @@
       <c r="K202" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L202">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>497</v>
       </c>
@@ -10480,8 +10495,11 @@
       <c r="K203" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L203">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>500</v>
       </c>
@@ -10515,8 +10533,11 @@
       <c r="K204" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L204">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>502</v>
       </c>
@@ -10550,8 +10571,11 @@
       <c r="K205" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L205">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>504</v>
       </c>
@@ -10585,8 +10609,11 @@
       <c r="K206" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L206">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>506</v>
       </c>
@@ -10620,8 +10647,11 @@
       <c r="K207" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L207">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>509</v>
       </c>
@@ -10655,8 +10685,11 @@
       <c r="K208" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L208">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>511</v>
       </c>
@@ -10690,8 +10723,11 @@
       <c r="K209" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L209">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>513</v>
       </c>
@@ -10725,8 +10761,11 @@
       <c r="K210" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L210">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>515</v>
       </c>
@@ -10760,8 +10799,11 @@
       <c r="K211" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L211">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>518</v>
       </c>
@@ -10795,8 +10837,11 @@
       <c r="K212" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L212">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>520</v>
       </c>
@@ -10830,8 +10875,11 @@
       <c r="K213" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L213">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>522</v>
       </c>
@@ -10865,8 +10913,11 @@
       <c r="K214" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L214">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>524</v>
       </c>
@@ -10900,8 +10951,11 @@
       <c r="K215" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L215">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>527</v>
       </c>
@@ -10935,8 +10989,11 @@
       <c r="K216" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L216">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>529</v>
       </c>
@@ -10970,8 +11027,11 @@
       <c r="K217" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L217">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>531</v>
       </c>
@@ -11005,8 +11065,11 @@
       <c r="K218" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L218">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>533</v>
       </c>
@@ -11040,8 +11103,11 @@
       <c r="K219" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L219">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>534</v>
       </c>
@@ -11075,8 +11141,11 @@
       <c r="K220" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L220">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>535</v>
       </c>
@@ -11110,8 +11179,11 @@
       <c r="K221" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L221">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>536</v>
       </c>
@@ -11145,8 +11217,11 @@
       <c r="K222" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L222">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>537</v>
       </c>
@@ -11180,8 +11255,11 @@
       <c r="K223" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L223">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>539</v>
       </c>
@@ -11215,8 +11293,11 @@
       <c r="K224" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L224">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>540</v>
       </c>
@@ -11250,8 +11331,11 @@
       <c r="K225" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L225">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>542</v>
       </c>
@@ -11285,8 +11369,11 @@
       <c r="K226" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L226">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>543</v>
       </c>
@@ -11320,8 +11407,11 @@
       <c r="K227" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L227">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>545</v>
       </c>
@@ -11355,8 +11445,11 @@
       <c r="K228" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L228">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>546</v>
       </c>
@@ -11390,8 +11483,11 @@
       <c r="K229" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L229">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>547</v>
       </c>
@@ -11425,8 +11521,11 @@
       <c r="K230" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L230">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>548</v>
       </c>
@@ -11460,8 +11559,11 @@
       <c r="K231" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L231">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>550</v>
       </c>
@@ -11495,8 +11597,11 @@
       <c r="K232" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L232">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>551</v>
       </c>
@@ -11530,8 +11635,11 @@
       <c r="K233" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L233">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>552</v>
       </c>
@@ -11565,8 +11673,11 @@
       <c r="K234" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L234">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>553</v>
       </c>
@@ -11600,8 +11711,11 @@
       <c r="K235" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L235">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>554</v>
       </c>
@@ -11635,8 +11749,11 @@
       <c r="K236" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L236">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>555</v>
       </c>
@@ -11670,8 +11787,11 @@
       <c r="K237" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L237">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>556</v>
       </c>
@@ -11705,8 +11825,11 @@
       <c r="K238" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L238">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>558</v>
       </c>
@@ -11740,8 +11863,11 @@
       <c r="K239" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L239">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>559</v>
       </c>
@@ -11775,8 +11901,11 @@
       <c r="K240" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L240">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>560</v>
       </c>
@@ -11810,8 +11939,11 @@
       <c r="K241" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L241">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>561</v>
       </c>
@@ -11845,8 +11977,11 @@
       <c r="K242" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L242">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>563</v>
       </c>
@@ -11880,8 +12015,11 @@
       <c r="K243" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L243">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>564</v>
       </c>
@@ -11915,8 +12053,11 @@
       <c r="K244" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L244">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>565</v>
       </c>
@@ -11950,8 +12091,11 @@
       <c r="K245" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L245">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>566</v>
       </c>
@@ -11985,8 +12129,11 @@
       <c r="K246" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L246">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>572</v>
       </c>
@@ -12020,8 +12167,11 @@
       <c r="K247" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L247">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>573</v>
       </c>
@@ -12055,8 +12205,11 @@
       <c r="K248" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L248">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>574</v>
       </c>
@@ -12090,8 +12243,11 @@
       <c r="K249" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L249">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>575</v>
       </c>
@@ -12125,8 +12281,11 @@
       <c r="K250" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L250">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>577</v>
       </c>
@@ -12160,8 +12319,11 @@
       <c r="K251" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L251">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>578</v>
       </c>
@@ -12195,8 +12357,11 @@
       <c r="K252" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L252">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>579</v>
       </c>
@@ -12230,8 +12395,11 @@
       <c r="K253" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L253">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>580</v>
       </c>
@@ -12265,8 +12433,11 @@
       <c r="K254" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L254">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>582</v>
       </c>
@@ -12300,8 +12471,11 @@
       <c r="K255" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L255">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>583</v>
       </c>
@@ -12335,8 +12509,11 @@
       <c r="K256" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L256">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>584</v>
       </c>
@@ -12370,8 +12547,11 @@
       <c r="K257" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L257">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>585</v>
       </c>
@@ -12405,8 +12585,11 @@
       <c r="K258" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L258">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>587</v>
       </c>
@@ -12440,8 +12623,11 @@
       <c r="K259" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L259">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>588</v>
       </c>
@@ -12475,8 +12661,11 @@
       <c r="K260" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L260">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>589</v>
       </c>
@@ -12510,8 +12699,11 @@
       <c r="K261" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L261">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>590</v>
       </c>
@@ -12545,8 +12737,11 @@
       <c r="K262" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L262">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>592</v>
       </c>
@@ -12580,8 +12775,11 @@
       <c r="K263" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L263">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>593</v>
       </c>
@@ -12615,8 +12813,11 @@
       <c r="K264" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L264">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>594</v>
       </c>
@@ -12650,8 +12851,11 @@
       <c r="K265" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L265">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>595</v>
       </c>
@@ -12685,8 +12889,11 @@
       <c r="K266" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L266">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>597</v>
       </c>
@@ -12720,8 +12927,11 @@
       <c r="K267" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L267">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>598</v>
       </c>
@@ -12755,8 +12965,11 @@
       <c r="K268" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L268">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>599</v>
       </c>
@@ -12790,8 +13003,11 @@
       <c r="K269" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L269">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>600</v>
       </c>
@@ -12825,8 +13041,11 @@
       <c r="K270" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L270">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>602</v>
       </c>
@@ -12860,8 +13079,11 @@
       <c r="K271" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L271">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>603</v>
       </c>
@@ -12895,8 +13117,11 @@
       <c r="K272" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L272">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>604</v>
       </c>
@@ -12930,8 +13155,11 @@
       <c r="K273" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L273">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>605</v>
       </c>
@@ -12965,8 +13193,11 @@
       <c r="K274" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L274">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>607</v>
       </c>
@@ -13000,8 +13231,11 @@
       <c r="K275" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L275">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>608</v>
       </c>
@@ -13035,8 +13269,11 @@
       <c r="K276" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L276">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>609</v>
       </c>
@@ -13070,8 +13307,11 @@
       <c r="K277" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L277">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>610</v>
       </c>
@@ -13105,8 +13345,11 @@
       <c r="K278" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L278">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>612</v>
       </c>
@@ -13140,8 +13383,11 @@
       <c r="K279" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L279">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>613</v>
       </c>
@@ -13175,8 +13421,11 @@
       <c r="K280" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L280">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>614</v>
       </c>
@@ -13210,8 +13459,11 @@
       <c r="K281" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L281">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>615</v>
       </c>
@@ -13245,8 +13497,11 @@
       <c r="K282" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L282">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>617</v>
       </c>
@@ -13280,8 +13535,11 @@
       <c r="K283" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L283">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>618</v>
       </c>
@@ -13315,8 +13573,11 @@
       <c r="K284" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L284">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>619</v>
       </c>
@@ -13350,8 +13611,11 @@
       <c r="K285" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L285">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>620</v>
       </c>
@@ -13385,8 +13649,11 @@
       <c r="K286" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L286">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>622</v>
       </c>
@@ -13420,8 +13687,11 @@
       <c r="K287" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L287">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>623</v>
       </c>
@@ -13455,8 +13725,11 @@
       <c r="K288" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L288">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>624</v>
       </c>
@@ -13490,8 +13763,11 @@
       <c r="K289" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L289">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>625</v>
       </c>
@@ -13525,8 +13801,11 @@
       <c r="K290" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L290">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>627</v>
       </c>
@@ -13560,8 +13839,11 @@
       <c r="K291" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L291">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>628</v>
       </c>
@@ -13595,8 +13877,11 @@
       <c r="K292" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L292">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>629</v>
       </c>
@@ -13630,8 +13915,11 @@
       <c r="K293" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L293">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>630</v>
       </c>
@@ -13665,8 +13953,11 @@
       <c r="K294" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L294">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="295" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>632</v>
       </c>
@@ -13700,8 +13991,11 @@
       <c r="K295" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L295">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>633</v>
       </c>
@@ -13735,8 +14029,11 @@
       <c r="K296" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L296">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>634</v>
       </c>
@@ -13770,8 +14067,11 @@
       <c r="K297" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L297">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>635</v>
       </c>
@@ -13805,8 +14105,11 @@
       <c r="K298" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L298">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>637</v>
       </c>
@@ -13840,8 +14143,11 @@
       <c r="K299" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L299">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>638</v>
       </c>
@@ -13875,8 +14181,11 @@
       <c r="K300" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L300">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>639</v>
       </c>
@@ -13910,8 +14219,11 @@
       <c r="K301" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L301">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>640</v>
       </c>
@@ -13945,8 +14257,11 @@
       <c r="K302" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L302">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>642</v>
       </c>
@@ -13980,8 +14295,11 @@
       <c r="K303" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L303">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>643</v>
       </c>
@@ -14015,8 +14333,11 @@
       <c r="K304" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L304">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>644</v>
       </c>
@@ -14050,8 +14371,11 @@
       <c r="K305" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L305">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>645</v>
       </c>
@@ -14085,8 +14409,11 @@
       <c r="K306" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L306">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>647</v>
       </c>
@@ -14120,8 +14447,11 @@
       <c r="K307" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L307">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>648</v>
       </c>
@@ -14155,8 +14485,11 @@
       <c r="K308" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L308">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>649</v>
       </c>
@@ -14190,8 +14523,11 @@
       <c r="K309" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L309">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>650</v>
       </c>
@@ -14225,8 +14561,11 @@
       <c r="K310" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L310">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="311" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>652</v>
       </c>
@@ -14260,8 +14599,11 @@
       <c r="K311" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L311">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>653</v>
       </c>
@@ -14295,8 +14637,11 @@
       <c r="K312" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L312">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>654</v>
       </c>
@@ -14330,8 +14675,11 @@
       <c r="K313" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L313">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>655</v>
       </c>
@@ -14365,8 +14713,11 @@
       <c r="K314" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L314">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>657</v>
       </c>
@@ -14400,8 +14751,11 @@
       <c r="K315" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L315">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>658</v>
       </c>
@@ -14435,8 +14789,11 @@
       <c r="K316" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L316">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>659</v>
       </c>
@@ -14470,8 +14827,11 @@
       <c r="K317" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L317">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="318" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>660</v>
       </c>
@@ -14505,8 +14865,11 @@
       <c r="K318" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L318">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>662</v>
       </c>
@@ -14540,8 +14903,11 @@
       <c r="K319" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L319">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="320" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>663</v>
       </c>
@@ -14575,8 +14941,11 @@
       <c r="K320" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L320">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="321" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>664</v>
       </c>
@@ -14610,8 +14979,11 @@
       <c r="K321" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L321">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="322" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>665</v>
       </c>
@@ -14645,8 +15017,11 @@
       <c r="K322" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L322">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="323" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>671</v>
       </c>
@@ -14680,8 +15055,11 @@
       <c r="K323" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L323">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="324" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>672</v>
       </c>
@@ -14715,8 +15093,11 @@
       <c r="K324" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L324">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="325" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>673</v>
       </c>
@@ -14750,8 +15131,11 @@
       <c r="K325" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L325">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="326" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>674</v>
       </c>
@@ -14785,8 +15169,11 @@
       <c r="K326" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L326">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="327" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>676</v>
       </c>
@@ -14820,8 +15207,11 @@
       <c r="K327" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L327">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="328" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>677</v>
       </c>
@@ -14855,8 +15245,11 @@
       <c r="K328" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L328">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="329" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>678</v>
       </c>
@@ -14890,8 +15283,11 @@
       <c r="K329" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L329">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="330" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>679</v>
       </c>
@@ -14925,8 +15321,11 @@
       <c r="K330" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L330">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="331" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>681</v>
       </c>
@@ -14960,8 +15359,11 @@
       <c r="K331" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L331">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="332" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>682</v>
       </c>
@@ -14995,8 +15397,11 @@
       <c r="K332" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L332">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="333" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>683</v>
       </c>
@@ -15030,8 +15435,11 @@
       <c r="K333" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L333">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="334" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>684</v>
       </c>
@@ -15065,8 +15473,11 @@
       <c r="K334" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L334">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="335" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>686</v>
       </c>
@@ -15100,8 +15511,11 @@
       <c r="K335" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L335">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="336" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>687</v>
       </c>
@@ -15135,8 +15549,11 @@
       <c r="K336" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L336">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="337" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>688</v>
       </c>
@@ -15170,8 +15587,11 @@
       <c r="K337" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L337">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="338" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>689</v>
       </c>
@@ -15205,8 +15625,11 @@
       <c r="K338" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L338">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="339" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>691</v>
       </c>
@@ -15240,8 +15663,11 @@
       <c r="K339" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L339">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="340" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>692</v>
       </c>
@@ -15275,8 +15701,11 @@
       <c r="K340" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L340">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="341" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>693</v>
       </c>
@@ -15310,8 +15739,11 @@
       <c r="K341" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L341">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="342" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>694</v>
       </c>
@@ -15345,8 +15777,11 @@
       <c r="K342" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L342">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="343" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>696</v>
       </c>
@@ -15380,8 +15815,11 @@
       <c r="K343" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L343">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="344" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>697</v>
       </c>
@@ -15415,8 +15853,11 @@
       <c r="K344" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L344">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="345" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>698</v>
       </c>
@@ -15450,8 +15891,11 @@
       <c r="K345" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L345">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="346" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>699</v>
       </c>
@@ -15485,8 +15929,11 @@
       <c r="K346" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L346">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="347" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>701</v>
       </c>
@@ -15520,8 +15967,11 @@
       <c r="K347" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L347">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="348" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>702</v>
       </c>
@@ -15555,8 +16005,11 @@
       <c r="K348" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L348">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="349" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>703</v>
       </c>
@@ -15590,8 +16043,11 @@
       <c r="K349" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L349">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="350" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>704</v>
       </c>
@@ -15625,8 +16081,11 @@
       <c r="K350" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L350">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="351" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>706</v>
       </c>
@@ -15660,8 +16119,11 @@
       <c r="K351" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L351">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="352" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>707</v>
       </c>
@@ -15695,8 +16157,11 @@
       <c r="K352" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L352">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="353" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>708</v>
       </c>
@@ -15730,8 +16195,11 @@
       <c r="K353" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L353">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="354" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>709</v>
       </c>
@@ -15765,8 +16233,11 @@
       <c r="K354" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L354">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="355" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>711</v>
       </c>
@@ -15800,8 +16271,11 @@
       <c r="K355" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L355">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="356" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>712</v>
       </c>
@@ -15835,8 +16309,11 @@
       <c r="K356" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L356">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="357" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>713</v>
       </c>
@@ -15870,8 +16347,11 @@
       <c r="K357" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L357">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="358" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>714</v>
       </c>
@@ -15905,8 +16385,11 @@
       <c r="K358" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L358">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="359" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>716</v>
       </c>
@@ -15940,8 +16423,11 @@
       <c r="K359" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L359">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="360" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>717</v>
       </c>
@@ -15975,8 +16461,11 @@
       <c r="K360" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L360">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="361" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>718</v>
       </c>
@@ -16010,8 +16499,11 @@
       <c r="K361" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L361">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="362" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>719</v>
       </c>
@@ -16045,8 +16537,11 @@
       <c r="K362" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L362">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="363" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>720</v>
       </c>
@@ -16080,8 +16575,11 @@
       <c r="K363" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L363">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="364" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>721</v>
       </c>
@@ -16115,8 +16613,11 @@
       <c r="K364" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L364">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="365" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>722</v>
       </c>
@@ -16150,8 +16651,11 @@
       <c r="K365" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L365">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="366" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>723</v>
       </c>
@@ -16185,8 +16689,11 @@
       <c r="K366" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L366">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="367" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>724</v>
       </c>
@@ -16220,8 +16727,11 @@
       <c r="K367" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L367">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="368" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>725</v>
       </c>
@@ -16255,8 +16765,11 @@
       <c r="K368" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L368">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="369" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
         <v>726</v>
       </c>
@@ -16290,8 +16803,11 @@
       <c r="K369" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L369">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="370" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
         <v>727</v>
       </c>
@@ -16325,8 +16841,11 @@
       <c r="K370" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L370">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="371" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
         <v>728</v>
       </c>
@@ -16360,8 +16879,11 @@
       <c r="K371" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L371">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="372" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
         <v>729</v>
       </c>
@@ -16395,8 +16917,11 @@
       <c r="K372" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L372">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="373" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
         <v>730</v>
       </c>
@@ -16430,8 +16955,11 @@
       <c r="K373" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L373">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="374" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
         <v>731</v>
       </c>
@@ -16465,8 +16993,11 @@
       <c r="K374" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L374">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="375" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
         <v>732</v>
       </c>
@@ -16500,8 +17031,11 @@
       <c r="K375" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L375">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="376" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
         <v>733</v>
       </c>
@@ -16535,8 +17069,11 @@
       <c r="K376" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L376">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="377" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
         <v>734</v>
       </c>
@@ -16570,8 +17107,11 @@
       <c r="K377" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L377">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="378" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
         <v>735</v>
       </c>
@@ -16605,8 +17145,11 @@
       <c r="K378" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L378">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="379" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
         <v>761</v>
       </c>
@@ -16641,7 +17184,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
         <v>762</v>
       </c>
@@ -16676,7 +17219,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
         <v>763</v>
       </c>
@@ -16711,7 +17254,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
         <v>764</v>
       </c>
@@ -16746,7 +17289,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
         <v>765</v>
       </c>
@@ -16781,7 +17324,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
         <v>766</v>
       </c>
@@ -17936,7 +18479,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="417" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
         <v>839</v>
       </c>
@@ -17971,7 +18514,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
         <v>840</v>
       </c>
@@ -18006,7 +18549,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
         <v>841</v>
       </c>
@@ -18041,7 +18584,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
         <v>842</v>
       </c>
@@ -18076,7 +18619,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
         <v>843</v>
       </c>
@@ -18111,7 +18654,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
         <v>881</v>
       </c>
@@ -18146,7 +18689,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="423" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
         <v>882</v>
       </c>
@@ -18181,7 +18724,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="424" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
         <v>887</v>
       </c>
@@ -18216,7 +18759,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="425" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
         <v>888</v>
       </c>
@@ -18251,7 +18794,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
         <v>892</v>
       </c>
@@ -18286,7 +18829,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="427" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
         <v>895</v>
       </c>
@@ -18321,7 +18864,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
         <v>897</v>
       </c>
@@ -18354,6 +18897,11 @@
       </c>
       <c r="K428" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="429" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L429" t="s">
+        <v>903</v>
       </c>
     </row>
   </sheetData>
@@ -18680,9 +19228,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18744,10 +19292,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>79</v>
+        <v>491</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.XLOOKUP(A2,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!F:F,"",0)</f>
@@ -18759,7 +19307,7 @@
       </c>
       <c r="E2" s="2">
         <f>_xlfn.XLOOKUP(A2,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
-        <v>415</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2">
         <f>_xlfn.XLOOKUP(D2,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
@@ -18767,11 +19315,11 @@
       </c>
       <c r="G2" s="7">
         <f>$E2*$F2</f>
-        <v>8715</v>
+        <v>210</v>
       </c>
       <c r="H2" s="8">
         <f>_xlfn.XLOOKUP($B$2,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="I2" s="8">
         <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -18795,11 +19343,11 @@
       </c>
       <c r="N2" s="2">
         <f>IF($C2="Importado",$G2*(1+$H2+I2+$J2+$L2+$M2),$G2)</f>
-        <v>9747.7275000000009</v>
+        <v>245.38500000000002</v>
       </c>
       <c r="O2" s="2">
         <f>N2 * (1 + K2)</f>
-        <v>10722.500250000001</v>
+        <v>269.92350000000005</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -18807,7 +19355,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C3" t="str">
         <f>_xlfn.XLOOKUP(A3,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!F:F,"",0)</f>
@@ -18831,7 +19379,7 @@
       </c>
       <c r="H3" s="8">
         <f>_xlfn.XLOOKUP($B$3,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I3" s="8">
         <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -18855,11 +19403,11 @@
       </c>
       <c r="N3" s="2">
         <f>IF($C3="Importado",$G3*(1+$H3+I3+$J3+$L3+$M3),$G3)</f>
-        <v>10183.477500000001</v>
+        <v>9747.7275000000009</v>
       </c>
       <c r="O3" s="2">
         <f>N3 * (1 + K3)</f>
-        <v>11201.825250000002</v>
+        <v>10722.500250000001</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -42831,7 +43379,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2890B5D1-F5C9-452F-8DA6-742FF446337F}">
           <x14:formula1>
             <xm:f>PARAMETROS_IMPORTACION!$A$2:$A$3</xm:f>

</xml_diff>

<commit_message>
docs: document changes (PDF layout, sequences, endpoints) and remove temp test artifacts
</commit_message>
<xml_diff>
--- a/Plantilla_Pricing_Costos_Importacion.xlsx
+++ b/Plantilla_Pricing_Costos_Importacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FernandoOlveraRendon\Documents\Base_Costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D65DC64-6083-471C-A978-5ECA7A7F8F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D71FF-9D36-42AB-AB33-A55976D23838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CATALOGO_PRODUCTOS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3921" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3929" uniqueCount="904">
   <si>
     <t>SKU</t>
   </si>
@@ -2831,6 +2831,7 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3349,7 +3350,7 @@
   </sheetPr>
   <dimension ref="A1:L429"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -19228,9 +19229,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O2000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19292,10 +19293,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>491</v>
+        <v>572</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.XLOOKUP(A2,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!F:F,"",0)</f>
@@ -19307,7 +19308,7 @@
       </c>
       <c r="E2" s="2">
         <f>_xlfn.XLOOKUP(A2,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2">
         <f>_xlfn.XLOOKUP(D2,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
@@ -19315,11 +19316,11 @@
       </c>
       <c r="G2" s="7">
         <f>$E2*$F2</f>
-        <v>210</v>
+        <v>273</v>
       </c>
       <c r="H2" s="8">
         <f>_xlfn.XLOOKUP($B$2,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I2" s="8">
         <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -19343,16 +19344,16 @@
       </c>
       <c r="N2" s="2">
         <f>IF($C2="Importado",$G2*(1+$H2+I2+$J2+$L2+$M2),$G2)</f>
-        <v>245.38500000000002</v>
+        <v>305.35050000000001</v>
       </c>
       <c r="O2" s="2">
         <f>N2 * (1 + K2)</f>
-        <v>269.92350000000005</v>
+        <v>335.88555000000002</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>577</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>162</v>
@@ -19367,7 +19368,7 @@
       </c>
       <c r="E3" s="2">
         <f>_xlfn.XLOOKUP(A3,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
-        <v>415</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2">
         <f>_xlfn.XLOOKUP(D3,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
@@ -19375,7 +19376,7 @@
       </c>
       <c r="G3" s="7">
         <f>$E3*$F3</f>
-        <v>8715</v>
+        <v>294</v>
       </c>
       <c r="H3" s="8">
         <f>_xlfn.XLOOKUP($B$3,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -19403,60 +19404,252 @@
       </c>
       <c r="N3" s="2">
         <f>IF($C3="Importado",$G3*(1+$H3+I3+$J3+$L3+$M3),$G3)</f>
-        <v>9747.7275000000009</v>
+        <v>328.839</v>
       </c>
       <c r="O3" s="2">
         <f>N3 * (1 + K3)</f>
-        <v>10722.500250000001</v>
+        <v>361.72290000000004</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="A4" t="s">
+        <v>762</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" t="str">
+        <f>_xlfn.XLOOKUP(A4,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!F:F,"",0)</f>
+        <v>Importado</v>
+      </c>
+      <c r="D4" t="str">
+        <f>_xlfn.XLOOKUP(A4,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!I:I,"",0)</f>
+        <v>USD</v>
+      </c>
+      <c r="E4" s="2">
+        <f>_xlfn.XLOOKUP(A4,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
+        <v>886</v>
+      </c>
+      <c r="F4" s="2">
+        <f>_xlfn.XLOOKUP(D4,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
+        <v>21</v>
+      </c>
+      <c r="G4" s="7">
+        <f>$E4*$F4</f>
+        <v>18606</v>
+      </c>
+      <c r="H4" s="8">
+        <f>_xlfn.XLOOKUP($B$4,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.05</v>
+      </c>
+      <c r="I4" s="8">
+        <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J4" s="8">
+        <f>_xlfn.XLOOKUP("Arancel",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.05</v>
+      </c>
+      <c r="K4" s="8">
+        <f>_xlfn.XLOOKUP("Mark_up",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="8">
+        <f>_xlfn.XLOOKUP("DTA",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="M4" s="11">
+        <f>_xlfn.XLOOKUP("Honorarios_Aduanales",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="N4" s="2">
+        <f>IF($C4="Importado",$G4*(1+$H4+I4+$J4+$L4+$M4),$G4)</f>
+        <v>20810.811000000002</v>
+      </c>
+      <c r="O4" s="2">
+        <f>N4 * (1 + K4)</f>
+        <v>22891.892100000005</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="A5" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xlfn.XLOOKUP(A5,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!F:F,"",0)</f>
+        <v>Importado</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xlfn.XLOOKUP(A5,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!I:I,"",0)</f>
+        <v>USD</v>
+      </c>
+      <c r="E5" s="2">
+        <f>_xlfn.XLOOKUP(A5,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
+        <v>13</v>
+      </c>
+      <c r="F5" s="2">
+        <f>_xlfn.XLOOKUP(D5,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
+        <v>21</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:G7" si="0">$E5*$F5</f>
+        <v>273</v>
+      </c>
+      <c r="H5" s="8">
+        <f>_xlfn.XLOOKUP($B$5,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="8">
+        <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J5" s="8">
+        <f>_xlfn.XLOOKUP("Arancel",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.05</v>
+      </c>
+      <c r="K5" s="8">
+        <f>_xlfn.XLOOKUP("Mark_up",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.1</v>
+      </c>
+      <c r="L5" s="8">
+        <f>_xlfn.XLOOKUP("DTA",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="M5" s="11">
+        <f>_xlfn.XLOOKUP("Honorarios_Aduanales",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" ref="N5:N7" si="1">IF($C5="Importado",$G5*(1+$H5+I5+$J5+$L5+$M5),$G5)</f>
+        <v>319.00050000000005</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" ref="O5:O7" si="2">N5 * (1 + K5)</f>
+        <v>350.90055000000007</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="A6" t="s">
+        <v>577</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xlfn.XLOOKUP(A6,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!F:F,"",0)</f>
+        <v>Importado</v>
+      </c>
+      <c r="D6" t="str">
+        <f>_xlfn.XLOOKUP(A6,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!I:I,"",0)</f>
+        <v>USD</v>
+      </c>
+      <c r="E6" s="2">
+        <f>_xlfn.XLOOKUP(A6,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
+        <v>14</v>
+      </c>
+      <c r="F6" s="2">
+        <f>_xlfn.XLOOKUP(D6,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
+        <v>21</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>294</v>
+      </c>
+      <c r="H6" s="8">
+        <f>_xlfn.XLOOKUP($B$6,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="8">
+        <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J6" s="8">
+        <f>_xlfn.XLOOKUP("Arancel",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.05</v>
+      </c>
+      <c r="K6" s="8">
+        <f>_xlfn.XLOOKUP("Mark_up",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.1</v>
+      </c>
+      <c r="L6" s="8">
+        <f>_xlfn.XLOOKUP("DTA",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="M6" s="11">
+        <f>_xlfn.XLOOKUP("Honorarios_Aduanales",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="1"/>
+        <v>343.53900000000004</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="2"/>
+        <v>377.89290000000005</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="A7" t="s">
+        <v>762</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" t="str">
+        <f>_xlfn.XLOOKUP(A7,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!F:F,"",0)</f>
+        <v>Importado</v>
+      </c>
+      <c r="D7" t="str">
+        <f>_xlfn.XLOOKUP(A7,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!I:I,"",0)</f>
+        <v>USD</v>
+      </c>
+      <c r="E7" s="2">
+        <f>_xlfn.XLOOKUP(A7,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
+        <v>886</v>
+      </c>
+      <c r="F7" s="2">
+        <f>_xlfn.XLOOKUP(D7,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
+        <v>21</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>18606</v>
+      </c>
+      <c r="H7" s="8">
+        <f>_xlfn.XLOOKUP($B$7,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="8">
+        <f>_xlfn.XLOOKUP("Seguro",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J7" s="8">
+        <f>_xlfn.XLOOKUP("Arancel",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.05</v>
+      </c>
+      <c r="K7" s="8">
+        <f>_xlfn.XLOOKUP("Mark_up",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="8">
+        <f>_xlfn.XLOOKUP("DTA",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="M7" s="11">
+        <f>_xlfn.XLOOKUP("Honorarios_Aduanales",PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="1"/>
+        <v>21741.111000000001</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="2"/>
+        <v>23915.222100000003</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E8" s="2"/>
@@ -43379,12 +43572,12 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2890B5D1-F5C9-452F-8DA6-742FF446337F}">
           <x14:formula1>
             <xm:f>PARAMETROS_IMPORTACION!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
+          <xm:sqref>B2:B7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
chore(clean): remove test artifacts and caches via tools/cleanup_repo.ps1
</commit_message>
<xml_diff>
--- a/Plantilla_Pricing_Costos_Importacion.xlsx
+++ b/Plantilla_Pricing_Costos_Importacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FernandoOlveraRendon\Documents\Base_Costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D71FF-9D36-42AB-AB33-A55976D23838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7386DEF-D6D9-4C42-B6DF-57725AF40F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="15810" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CATALOGO_PRODUCTOS" sheetId="1" r:id="rId1"/>
@@ -2818,7 +2818,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2860,6 +2860,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2893,7 +2900,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2912,6 +2919,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
@@ -2971,7 +2979,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>400</xdr:row>
+      <xdr:row>432</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3014,6 +3022,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblCatalogo" displayName="tblCatalogo" ref="A1:K428" headerRowCellStyle="Normal" dataCellStyle="Normal" totalsRowCellStyle="Normal">
+  <autoFilter ref="A1:K428" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="D0031"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K197">
     <sortCondition sortBy="fontColor" ref="A1:A197" dxfId="4"/>
   </sortState>
@@ -3352,7 +3367,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3447,7 +3462,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>304</v>
       </c>
@@ -3482,7 +3497,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>305</v>
       </c>
@@ -3517,7 +3532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>306</v>
       </c>
@@ -3552,7 +3567,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>307</v>
       </c>
@@ -3587,7 +3602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -3622,7 +3637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -3657,7 +3672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>254</v>
       </c>
@@ -3692,7 +3707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>255</v>
       </c>
@@ -3727,7 +3742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>256</v>
       </c>
@@ -3762,7 +3777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>258</v>
       </c>
@@ -3797,7 +3812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>259</v>
       </c>
@@ -3832,7 +3847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>469</v>
       </c>
@@ -3867,7 +3882,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>471</v>
       </c>
@@ -3905,7 +3920,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>472</v>
       </c>
@@ -3940,7 +3955,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>473</v>
       </c>
@@ -3975,7 +3990,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>474</v>
       </c>
@@ -4010,7 +4025,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -4045,7 +4060,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>138</v>
       </c>
@@ -4080,7 +4095,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>135</v>
       </c>
@@ -4115,7 +4130,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -4150,7 +4165,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>115</v>
       </c>
@@ -4185,7 +4200,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -4220,7 +4235,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -4255,7 +4270,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -4290,7 +4305,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -4325,7 +4340,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -4360,7 +4375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>144</v>
       </c>
@@ -4395,7 +4410,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -4430,7 +4445,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -4465,7 +4480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -4500,7 +4515,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -4535,7 +4550,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -4570,7 +4585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -4605,7 +4620,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -4640,7 +4655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -4675,7 +4690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -4710,7 +4725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -4745,7 +4760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -4780,7 +4795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -4815,7 +4830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -4850,7 +4865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -4885,7 +4900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -4920,7 +4935,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -4955,7 +4970,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -4990,7 +5005,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -5025,7 +5040,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -5060,7 +5075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -5095,7 +5110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>147</v>
       </c>
@@ -5130,7 +5145,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -5165,7 +5180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>431</v>
       </c>
@@ -5200,7 +5215,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -5235,7 +5250,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>434</v>
       </c>
@@ -5270,7 +5285,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>448</v>
       </c>
@@ -5305,7 +5320,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>446</v>
       </c>
@@ -5340,7 +5355,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>440</v>
       </c>
@@ -5375,7 +5390,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>442</v>
       </c>
@@ -5410,7 +5425,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>444</v>
       </c>
@@ -5445,7 +5460,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>439</v>
       </c>
@@ -5480,7 +5495,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>456</v>
       </c>
@@ -5515,7 +5530,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>459</v>
       </c>
@@ -5550,7 +5565,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>266</v>
       </c>
@@ -5585,7 +5600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>267</v>
       </c>
@@ -5620,7 +5635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>268</v>
       </c>
@@ -5655,7 +5670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>269</v>
       </c>
@@ -5690,7 +5705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>264</v>
       </c>
@@ -5725,7 +5740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>265</v>
       </c>
@@ -5760,7 +5775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>261</v>
       </c>
@@ -5795,7 +5810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>262</v>
       </c>
@@ -5830,7 +5845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>263</v>
       </c>
@@ -5865,7 +5880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>191</v>
       </c>
@@ -5900,7 +5915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>192</v>
       </c>
@@ -5935,7 +5950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>193</v>
       </c>
@@ -5970,7 +5985,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>260</v>
       </c>
@@ -6005,7 +6020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>189</v>
       </c>
@@ -6040,7 +6055,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>190</v>
       </c>
@@ -6075,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>275</v>
       </c>
@@ -6110,7 +6125,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>276</v>
       </c>
@@ -6145,7 +6160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>277</v>
       </c>
@@ -6180,7 +6195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>272</v>
       </c>
@@ -6215,7 +6230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>273</v>
       </c>
@@ -6250,7 +6265,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>274</v>
       </c>
@@ -6285,7 +6300,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>270</v>
       </c>
@@ -6320,7 +6335,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>271</v>
       </c>
@@ -6355,7 +6370,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>283</v>
       </c>
@@ -6390,7 +6405,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>280</v>
       </c>
@@ -6425,7 +6440,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>281</v>
       </c>
@@ -6460,7 +6475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>282</v>
       </c>
@@ -6495,7 +6510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>278</v>
       </c>
@@ -6530,7 +6545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>279</v>
       </c>
@@ -6565,7 +6580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>286</v>
       </c>
@@ -6600,7 +6615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>287</v>
       </c>
@@ -6635,7 +6650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>288</v>
       </c>
@@ -6670,7 +6685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>285</v>
       </c>
@@ -6705,7 +6720,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>284</v>
       </c>
@@ -6740,7 +6755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>294</v>
       </c>
@@ -6775,7 +6790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>295</v>
       </c>
@@ -6810,7 +6825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>291</v>
       </c>
@@ -6845,7 +6860,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>292</v>
       </c>
@@ -6880,7 +6895,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>293</v>
       </c>
@@ -6915,7 +6930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>289</v>
       </c>
@@ -6950,7 +6965,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>290</v>
       </c>
@@ -6985,7 +7000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>301</v>
       </c>
@@ -7020,7 +7035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>302</v>
       </c>
@@ -7055,7 +7070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>298</v>
       </c>
@@ -7090,7 +7105,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>299</v>
       </c>
@@ -7125,7 +7140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>300</v>
       </c>
@@ -7160,7 +7175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>296</v>
       </c>
@@ -7195,7 +7210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>297</v>
       </c>
@@ -7230,7 +7245,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>251</v>
       </c>
@@ -7265,7 +7280,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>252</v>
       </c>
@@ -7300,7 +7315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>207</v>
       </c>
@@ -7335,7 +7350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>208</v>
       </c>
@@ -7370,7 +7385,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>209</v>
       </c>
@@ -7405,7 +7420,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>210</v>
       </c>
@@ -7440,7 +7455,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>205</v>
       </c>
@@ -7475,7 +7490,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>206</v>
       </c>
@@ -7510,7 +7525,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>202</v>
       </c>
@@ -7545,7 +7560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>203</v>
       </c>
@@ -7580,7 +7595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>204</v>
       </c>
@@ -7615,7 +7630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>200</v>
       </c>
@@ -7650,7 +7665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>201</v>
       </c>
@@ -7685,7 +7700,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>196</v>
       </c>
@@ -7720,7 +7735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>197</v>
       </c>
@@ -7755,7 +7770,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>198</v>
       </c>
@@ -7790,7 +7805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>199</v>
       </c>
@@ -7825,7 +7840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>194</v>
       </c>
@@ -7860,7 +7875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>195</v>
       </c>
@@ -7895,7 +7910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>221</v>
       </c>
@@ -7930,7 +7945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>222</v>
       </c>
@@ -7965,7 +7980,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>223</v>
       </c>
@@ -8000,7 +8015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>219</v>
       </c>
@@ -8035,7 +8050,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>220</v>
       </c>
@@ -8070,7 +8085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>217</v>
       </c>
@@ -8105,7 +8120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>218</v>
       </c>
@@ -8140,7 +8155,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>215</v>
       </c>
@@ -8175,7 +8190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>216</v>
       </c>
@@ -8210,7 +8225,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>211</v>
       </c>
@@ -8245,7 +8260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>212</v>
       </c>
@@ -8280,7 +8295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>213</v>
       </c>
@@ -8315,7 +8330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>214</v>
       </c>
@@ -8350,7 +8365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>229</v>
       </c>
@@ -8385,7 +8400,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>226</v>
       </c>
@@ -8420,7 +8435,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>227</v>
       </c>
@@ -8455,7 +8470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>228</v>
       </c>
@@ -8490,7 +8505,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>224</v>
       </c>
@@ -8525,7 +8540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>225</v>
       </c>
@@ -8560,7 +8575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>236</v>
       </c>
@@ -8595,7 +8610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>237</v>
       </c>
@@ -8630,7 +8645,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>238</v>
       </c>
@@ -8665,7 +8680,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>234</v>
       </c>
@@ -8700,7 +8715,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>235</v>
       </c>
@@ -8735,7 +8750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>233</v>
       </c>
@@ -8770,7 +8785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>230</v>
       </c>
@@ -8805,7 +8820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>231</v>
       </c>
@@ -8840,7 +8855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>232</v>
       </c>
@@ -8875,7 +8890,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>257</v>
       </c>
@@ -8910,7 +8925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>242</v>
       </c>
@@ -8945,7 +8960,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>243</v>
       </c>
@@ -8980,7 +8995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>244</v>
       </c>
@@ -9015,7 +9030,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>240</v>
       </c>
@@ -9050,7 +9065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>241</v>
       </c>
@@ -9085,7 +9100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>239</v>
       </c>
@@ -9120,7 +9135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>248</v>
       </c>
@@ -9155,7 +9170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>249</v>
       </c>
@@ -9190,7 +9205,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>250</v>
       </c>
@@ -9225,7 +9240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>246</v>
       </c>
@@ -9260,7 +9275,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>247</v>
       </c>
@@ -9295,7 +9310,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>245</v>
       </c>
@@ -9330,7 +9345,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>81</v>
       </c>
@@ -9365,7 +9380,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>453</v>
       </c>
@@ -9400,7 +9415,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>79</v>
       </c>
@@ -9435,7 +9450,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>119</v>
       </c>
@@ -9470,7 +9485,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>82</v>
       </c>
@@ -9505,7 +9520,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>85</v>
       </c>
@@ -9540,7 +9555,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>122</v>
       </c>
@@ -9575,7 +9590,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>75</v>
       </c>
@@ -9610,7 +9625,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>124</v>
       </c>
@@ -9645,7 +9660,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>72</v>
       </c>
@@ -9680,7 +9695,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>127</v>
       </c>
@@ -9715,7 +9730,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>487</v>
       </c>
@@ -9750,7 +9765,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>91</v>
       </c>
@@ -9785,7 +9800,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>463</v>
       </c>
@@ -9820,7 +9835,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>461</v>
       </c>
@@ -9855,7 +9870,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>438</v>
       </c>
@@ -9890,7 +9905,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>450</v>
       </c>
@@ -9925,7 +9940,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>97</v>
       </c>
@@ -9960,7 +9975,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>88</v>
       </c>
@@ -9995,7 +10010,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>149</v>
       </c>
@@ -10030,7 +10045,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:11" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>466</v>
       </c>
@@ -10065,7 +10080,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>132</v>
       </c>
@@ -10100,7 +10115,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>129</v>
       </c>
@@ -10135,7 +10150,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>68</v>
       </c>
@@ -10170,7 +10185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>64</v>
       </c>
@@ -10205,7 +10220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>150</v>
       </c>
@@ -10240,7 +10255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>153</v>
       </c>
@@ -10275,7 +10290,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>485</v>
       </c>
@@ -10310,7 +10325,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>488</v>
       </c>
@@ -10348,7 +10363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>491</v>
       </c>
@@ -10386,7 +10401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>493</v>
       </c>
@@ -10424,7 +10439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>495</v>
       </c>
@@ -10462,7 +10477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>497</v>
       </c>
@@ -10500,7 +10515,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>500</v>
       </c>
@@ -10538,7 +10553,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>502</v>
       </c>
@@ -10576,7 +10591,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>504</v>
       </c>
@@ -10614,7 +10629,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>506</v>
       </c>
@@ -10652,7 +10667,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>509</v>
       </c>
@@ -10690,7 +10705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>511</v>
       </c>
@@ -10728,7 +10743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>513</v>
       </c>
@@ -10766,7 +10781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>515</v>
       </c>
@@ -10804,7 +10819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>518</v>
       </c>
@@ -10842,7 +10857,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>520</v>
       </c>
@@ -10880,7 +10895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>522</v>
       </c>
@@ -10918,7 +10933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>524</v>
       </c>
@@ -10956,7 +10971,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>527</v>
       </c>
@@ -10994,7 +11009,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>529</v>
       </c>
@@ -11032,7 +11047,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>531</v>
       </c>
@@ -11070,7 +11085,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>533</v>
       </c>
@@ -11108,7 +11123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>534</v>
       </c>
@@ -11146,7 +11161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>535</v>
       </c>
@@ -11184,7 +11199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>536</v>
       </c>
@@ -11222,7 +11237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>537</v>
       </c>
@@ -11260,7 +11275,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>539</v>
       </c>
@@ -11298,7 +11313,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>540</v>
       </c>
@@ -11336,7 +11351,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>542</v>
       </c>
@@ -11374,7 +11389,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>543</v>
       </c>
@@ -11412,7 +11427,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>545</v>
       </c>
@@ -11450,7 +11465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>546</v>
       </c>
@@ -11488,7 +11503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>547</v>
       </c>
@@ -11526,7 +11541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>548</v>
       </c>
@@ -11564,7 +11579,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>550</v>
       </c>
@@ -11602,7 +11617,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>551</v>
       </c>
@@ -11640,7 +11655,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>552</v>
       </c>
@@ -11678,7 +11693,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>553</v>
       </c>
@@ -11716,7 +11731,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>554</v>
       </c>
@@ -11754,7 +11769,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>555</v>
       </c>
@@ -11792,7 +11807,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>556</v>
       </c>
@@ -11830,7 +11845,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>558</v>
       </c>
@@ -11868,7 +11883,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>559</v>
       </c>
@@ -11906,7 +11921,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>560</v>
       </c>
@@ -11944,7 +11959,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>561</v>
       </c>
@@ -11982,7 +11997,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>563</v>
       </c>
@@ -12020,7 +12035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>564</v>
       </c>
@@ -12058,7 +12073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>565</v>
       </c>
@@ -12096,7 +12111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>566</v>
       </c>
@@ -12134,7 +12149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>572</v>
       </c>
@@ -12172,7 +12187,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>573</v>
       </c>
@@ -12210,7 +12225,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>574</v>
       </c>
@@ -12248,7 +12263,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>575</v>
       </c>
@@ -12286,7 +12301,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>577</v>
       </c>
@@ -12324,7 +12339,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>578</v>
       </c>
@@ -12362,7 +12377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>579</v>
       </c>
@@ -12400,7 +12415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>580</v>
       </c>
@@ -12438,7 +12453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>582</v>
       </c>
@@ -12476,7 +12491,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>583</v>
       </c>
@@ -12514,7 +12529,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>584</v>
       </c>
@@ -12552,7 +12567,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>585</v>
       </c>
@@ -12590,7 +12605,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>587</v>
       </c>
@@ -12628,7 +12643,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>588</v>
       </c>
@@ -12666,7 +12681,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>589</v>
       </c>
@@ -12704,7 +12719,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>590</v>
       </c>
@@ -12742,7 +12757,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>592</v>
       </c>
@@ -12780,7 +12795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>593</v>
       </c>
@@ -12818,7 +12833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>594</v>
       </c>
@@ -12856,7 +12871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>595</v>
       </c>
@@ -12894,7 +12909,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>597</v>
       </c>
@@ -12932,7 +12947,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>598</v>
       </c>
@@ -12970,7 +12985,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>599</v>
       </c>
@@ -13008,7 +13023,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>600</v>
       </c>
@@ -13046,7 +13061,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>602</v>
       </c>
@@ -13084,7 +13099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>603</v>
       </c>
@@ -13122,7 +13137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>604</v>
       </c>
@@ -13160,7 +13175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>605</v>
       </c>
@@ -13198,7 +13213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>607</v>
       </c>
@@ -13236,7 +13251,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>608</v>
       </c>
@@ -13274,7 +13289,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>609</v>
       </c>
@@ -13312,7 +13327,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>610</v>
       </c>
@@ -13350,7 +13365,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>612</v>
       </c>
@@ -13388,7 +13403,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>613</v>
       </c>
@@ -13426,7 +13441,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>614</v>
       </c>
@@ -13464,7 +13479,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>615</v>
       </c>
@@ -13502,7 +13517,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>617</v>
       </c>
@@ -13540,7 +13555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>618</v>
       </c>
@@ -13578,7 +13593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>619</v>
       </c>
@@ -13616,7 +13631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>620</v>
       </c>
@@ -13654,7 +13669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>622</v>
       </c>
@@ -13692,7 +13707,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>623</v>
       </c>
@@ -13730,7 +13745,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>624</v>
       </c>
@@ -13768,7 +13783,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>625</v>
       </c>
@@ -13806,7 +13821,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>627</v>
       </c>
@@ -13844,7 +13859,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>628</v>
       </c>
@@ -13882,7 +13897,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>629</v>
       </c>
@@ -13920,7 +13935,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>630</v>
       </c>
@@ -13958,7 +13973,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>632</v>
       </c>
@@ -13996,7 +14011,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>633</v>
       </c>
@@ -14034,7 +14049,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>634</v>
       </c>
@@ -14072,7 +14087,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>635</v>
       </c>
@@ -14110,7 +14125,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>637</v>
       </c>
@@ -14148,7 +14163,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>638</v>
       </c>
@@ -14186,7 +14201,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>639</v>
       </c>
@@ -14224,7 +14239,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>640</v>
       </c>
@@ -14262,7 +14277,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>642</v>
       </c>
@@ -14300,7 +14315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>643</v>
       </c>
@@ -14338,7 +14353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>644</v>
       </c>
@@ -14376,7 +14391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>645</v>
       </c>
@@ -14414,7 +14429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>647</v>
       </c>
@@ -14452,7 +14467,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>648</v>
       </c>
@@ -14490,7 +14505,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>649</v>
       </c>
@@ -14528,7 +14543,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>650</v>
       </c>
@@ -14566,7 +14581,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>652</v>
       </c>
@@ -14604,7 +14619,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>653</v>
       </c>
@@ -14642,7 +14657,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>654</v>
       </c>
@@ -14680,7 +14695,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>655</v>
       </c>
@@ -14718,7 +14733,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>657</v>
       </c>
@@ -14756,7 +14771,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>658</v>
       </c>
@@ -14794,7 +14809,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>659</v>
       </c>
@@ -14832,7 +14847,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>660</v>
       </c>
@@ -14870,7 +14885,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>662</v>
       </c>
@@ -14908,7 +14923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>663</v>
       </c>
@@ -14946,7 +14961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>664</v>
       </c>
@@ -14984,7 +14999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>665</v>
       </c>
@@ -15022,7 +15037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>671</v>
       </c>
@@ -15060,7 +15075,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>672</v>
       </c>
@@ -15098,7 +15113,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>673</v>
       </c>
@@ -15136,7 +15151,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>674</v>
       </c>
@@ -15174,7 +15189,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>676</v>
       </c>
@@ -15212,7 +15227,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>677</v>
       </c>
@@ -15250,7 +15265,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>678</v>
       </c>
@@ -15288,7 +15303,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>679</v>
       </c>
@@ -15326,7 +15341,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>681</v>
       </c>
@@ -15364,7 +15379,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>682</v>
       </c>
@@ -15402,7 +15417,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>683</v>
       </c>
@@ -15440,7 +15455,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>684</v>
       </c>
@@ -15478,7 +15493,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>686</v>
       </c>
@@ -15516,7 +15531,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>687</v>
       </c>
@@ -15554,7 +15569,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>688</v>
       </c>
@@ -15592,7 +15607,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>689</v>
       </c>
@@ -15630,7 +15645,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>691</v>
       </c>
@@ -15668,7 +15683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>692</v>
       </c>
@@ -15706,7 +15721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>693</v>
       </c>
@@ -15744,7 +15759,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>694</v>
       </c>
@@ -15782,7 +15797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>696</v>
       </c>
@@ -15820,7 +15835,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>697</v>
       </c>
@@ -15858,7 +15873,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="345" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>698</v>
       </c>
@@ -15896,7 +15911,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="346" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>699</v>
       </c>
@@ -15934,7 +15949,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="347" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>701</v>
       </c>
@@ -15972,7 +15987,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="348" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>702</v>
       </c>
@@ -16010,7 +16025,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="349" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>703</v>
       </c>
@@ -16048,7 +16063,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="350" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>704</v>
       </c>
@@ -16086,7 +16101,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="351" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>706</v>
       </c>
@@ -16124,7 +16139,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="352" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>707</v>
       </c>
@@ -16162,7 +16177,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="353" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>708</v>
       </c>
@@ -16200,7 +16215,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="354" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>709</v>
       </c>
@@ -16238,7 +16253,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="355" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>711</v>
       </c>
@@ -16276,7 +16291,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="356" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>712</v>
       </c>
@@ -16314,7 +16329,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="357" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>713</v>
       </c>
@@ -16352,7 +16367,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="358" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>714</v>
       </c>
@@ -16390,7 +16405,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="359" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>716</v>
       </c>
@@ -16428,7 +16443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="360" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>717</v>
       </c>
@@ -16466,7 +16481,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="361" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>718</v>
       </c>
@@ -16504,7 +16519,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="362" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>719</v>
       </c>
@@ -16542,7 +16557,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="363" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>720</v>
       </c>
@@ -16580,7 +16595,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="364" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>721</v>
       </c>
@@ -16618,7 +16633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="365" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>722</v>
       </c>
@@ -16656,7 +16671,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="366" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>723</v>
       </c>
@@ -16694,7 +16709,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="367" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>724</v>
       </c>
@@ -16732,7 +16747,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="368" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>725</v>
       </c>
@@ -16770,7 +16785,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
         <v>726</v>
       </c>
@@ -16808,7 +16823,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
         <v>727</v>
       </c>
@@ -16846,7 +16861,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
         <v>728</v>
       </c>
@@ -16884,7 +16899,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
         <v>729</v>
       </c>
@@ -16922,7 +16937,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
         <v>730</v>
       </c>
@@ -16960,7 +16975,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
         <v>731</v>
       </c>
@@ -16998,7 +17013,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
         <v>732</v>
       </c>
@@ -17036,7 +17051,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
         <v>733</v>
       </c>
@@ -17074,7 +17089,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
         <v>734</v>
       </c>
@@ -17112,7 +17127,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
         <v>735</v>
       </c>
@@ -17150,7 +17165,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
         <v>761</v>
       </c>
@@ -17185,7 +17200,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
         <v>762</v>
       </c>
@@ -17220,7 +17235,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
         <v>763</v>
       </c>
@@ -17255,7 +17270,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="382" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
         <v>764</v>
       </c>
@@ -17290,7 +17305,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
         <v>765</v>
       </c>
@@ -17325,7 +17340,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="384" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
         <v>766</v>
       </c>
@@ -17360,7 +17375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
         <v>767</v>
       </c>
@@ -17395,7 +17410,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
         <v>768</v>
       </c>
@@ -17430,7 +17445,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
         <v>769</v>
       </c>
@@ -17465,7 +17480,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
         <v>770</v>
       </c>
@@ -17500,7 +17515,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
         <v>771</v>
       </c>
@@ -17535,7 +17550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
         <v>772</v>
       </c>
@@ -17570,7 +17585,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
         <v>773</v>
       </c>
@@ -17605,7 +17620,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
         <v>774</v>
       </c>
@@ -17640,7 +17655,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
         <v>775</v>
       </c>
@@ -17675,7 +17690,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
         <v>776</v>
       </c>
@@ -17710,7 +17725,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
         <v>777</v>
       </c>
@@ -17745,7 +17760,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
         <v>778</v>
       </c>
@@ -17780,7 +17795,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
         <v>779</v>
       </c>
@@ -17815,7 +17830,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
         <v>810</v>
       </c>
@@ -17850,7 +17865,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
         <v>811</v>
       </c>
@@ -17885,7 +17900,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
         <v>812</v>
       </c>
@@ -17920,7 +17935,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
         <v>813</v>
       </c>
@@ -17955,7 +17970,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="402" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
         <v>814</v>
       </c>
@@ -17990,7 +18005,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
         <v>825</v>
       </c>
@@ -18025,7 +18040,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
         <v>826</v>
       </c>
@@ -18060,7 +18075,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
         <v>827</v>
       </c>
@@ -18095,7 +18110,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
         <v>828</v>
       </c>
@@ -18130,7 +18145,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
         <v>829</v>
       </c>
@@ -18165,7 +18180,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
         <v>830</v>
       </c>
@@ -18200,7 +18215,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
         <v>831</v>
       </c>
@@ -18235,7 +18250,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
         <v>832</v>
       </c>
@@ -18270,7 +18285,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
         <v>833</v>
       </c>
@@ -18305,7 +18320,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
         <v>834</v>
       </c>
@@ -18340,7 +18355,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
         <v>835</v>
       </c>
@@ -18375,7 +18390,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
         <v>836</v>
       </c>
@@ -18410,7 +18425,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="415" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
         <v>837</v>
       </c>
@@ -18445,7 +18460,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
         <v>838</v>
       </c>
@@ -18480,7 +18495,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="417" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
         <v>839</v>
       </c>
@@ -18515,7 +18530,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="418" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
         <v>840</v>
       </c>
@@ -18550,7 +18565,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="419" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
         <v>841</v>
       </c>
@@ -18585,7 +18600,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="420" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
         <v>842</v>
       </c>
@@ -18620,7 +18635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="421" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
         <v>843</v>
       </c>
@@ -18655,7 +18670,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="422" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
         <v>881</v>
       </c>
@@ -18690,7 +18705,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="423" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
         <v>882</v>
       </c>
@@ -18725,7 +18740,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="424" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
         <v>887</v>
       </c>
@@ -18760,7 +18775,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="425" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
         <v>888</v>
       </c>
@@ -18795,7 +18810,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="426" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
         <v>892</v>
       </c>
@@ -18830,7 +18845,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="427" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
         <v>895</v>
       </c>
@@ -18865,7 +18880,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="428" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
         <v>897</v>
       </c>
@@ -19231,7 +19246,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19292,8 +19307,8 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>572</v>
+      <c r="A2" s="12" t="s">
+        <v>303</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>162</v>
@@ -19308,7 +19323,7 @@
       </c>
       <c r="E2" s="2">
         <f>_xlfn.XLOOKUP(A2,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
-        <v>13</v>
+        <v>2.35E-2</v>
       </c>
       <c r="F2" s="2">
         <f>_xlfn.XLOOKUP(D2,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
@@ -19316,7 +19331,7 @@
       </c>
       <c r="G2" s="7">
         <f>$E2*$F2</f>
-        <v>273</v>
+        <v>0.49349999999999999</v>
       </c>
       <c r="H2" s="8">
         <f>_xlfn.XLOOKUP($B$2,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -19344,11 +19359,11 @@
       </c>
       <c r="N2" s="2">
         <f>IF($C2="Importado",$G2*(1+$H2+I2+$J2+$L2+$M2),$G2)</f>
-        <v>305.35050000000001</v>
+        <v>0.55197974999999999</v>
       </c>
       <c r="O2" s="2">
         <f>N2 * (1 + K2)</f>
-        <v>335.88555000000002</v>
+        <v>0.607177725</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Revert "chore(clean): remove test artifacts and caches via tools/cleanup_repo.ps1"
This reverts commit b1addf5bf3aca1d792797a7adeca77c4115b40b4.
</commit_message>
<xml_diff>
--- a/Plantilla_Pricing_Costos_Importacion.xlsx
+++ b/Plantilla_Pricing_Costos_Importacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FernandoOlveraRendon\Documents\Base_Costos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7386DEF-D6D9-4C42-B6DF-57725AF40F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D71FF-9D36-42AB-AB33-A55976D23838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="15810" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CATALOGO_PRODUCTOS" sheetId="1" r:id="rId1"/>
@@ -2818,7 +2818,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2860,13 +2860,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2900,7 +2893,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2919,7 +2912,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
@@ -2979,7 +2971,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>432</xdr:row>
+      <xdr:row>400</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3022,13 +3014,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblCatalogo" displayName="tblCatalogo" ref="A1:K428" headerRowCellStyle="Normal" dataCellStyle="Normal" totalsRowCellStyle="Normal">
-  <autoFilter ref="A1:K428" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="D0031"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K197">
     <sortCondition sortBy="fontColor" ref="A1:A197" dxfId="4"/>
   </sortState>
@@ -3367,7 +3352,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3462,7 +3447,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>304</v>
       </c>
@@ -3497,7 +3482,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>305</v>
       </c>
@@ -3532,7 +3517,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>306</v>
       </c>
@@ -3567,7 +3552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>307</v>
       </c>
@@ -3602,7 +3587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>308</v>
       </c>
@@ -3637,7 +3622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>253</v>
       </c>
@@ -3672,7 +3657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>254</v>
       </c>
@@ -3707,7 +3692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>255</v>
       </c>
@@ -3742,7 +3727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>256</v>
       </c>
@@ -3777,7 +3762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>258</v>
       </c>
@@ -3812,7 +3797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>259</v>
       </c>
@@ -3847,7 +3832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>469</v>
       </c>
@@ -3882,7 +3867,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>471</v>
       </c>
@@ -3920,7 +3905,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>472</v>
       </c>
@@ -3955,7 +3940,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>473</v>
       </c>
@@ -3990,7 +3975,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>474</v>
       </c>
@@ -4025,7 +4010,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -4060,7 +4045,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>138</v>
       </c>
@@ -4095,7 +4080,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>135</v>
       </c>
@@ -4130,7 +4115,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -4165,7 +4150,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>115</v>
       </c>
@@ -4200,7 +4185,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -4235,7 +4220,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -4270,7 +4255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -4305,7 +4290,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -4340,7 +4325,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -4375,7 +4360,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>144</v>
       </c>
@@ -4410,7 +4395,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -4445,7 +4430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -4480,7 +4465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -4515,7 +4500,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -4550,7 +4535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -4585,7 +4570,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -4620,7 +4605,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -4655,7 +4640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -4690,7 +4675,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -4725,7 +4710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -4760,7 +4745,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -4795,7 +4780,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -4830,7 +4815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -4865,7 +4850,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -4900,7 +4885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -4935,7 +4920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -4970,7 +4955,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -5005,7 +4990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -5040,7 +5025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -5075,7 +5060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -5110,7 +5095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>147</v>
       </c>
@@ -5145,7 +5130,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -5180,7 +5165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>431</v>
       </c>
@@ -5215,7 +5200,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -5250,7 +5235,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>434</v>
       </c>
@@ -5285,7 +5270,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>448</v>
       </c>
@@ -5320,7 +5305,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>446</v>
       </c>
@@ -5355,7 +5340,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>440</v>
       </c>
@@ -5390,7 +5375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>442</v>
       </c>
@@ -5425,7 +5410,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>444</v>
       </c>
@@ -5460,7 +5445,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>439</v>
       </c>
@@ -5495,7 +5480,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>456</v>
       </c>
@@ -5530,7 +5515,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>459</v>
       </c>
@@ -5565,7 +5550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>266</v>
       </c>
@@ -5600,7 +5585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>267</v>
       </c>
@@ -5635,7 +5620,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>268</v>
       </c>
@@ -5670,7 +5655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>269</v>
       </c>
@@ -5705,7 +5690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>264</v>
       </c>
@@ -5740,7 +5725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>265</v>
       </c>
@@ -5775,7 +5760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>261</v>
       </c>
@@ -5810,7 +5795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>262</v>
       </c>
@@ -5845,7 +5830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>263</v>
       </c>
@@ -5880,7 +5865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>191</v>
       </c>
@@ -5915,7 +5900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>192</v>
       </c>
@@ -5950,7 +5935,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>193</v>
       </c>
@@ -5985,7 +5970,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>260</v>
       </c>
@@ -6020,7 +6005,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>189</v>
       </c>
@@ -6055,7 +6040,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>190</v>
       </c>
@@ -6090,7 +6075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>275</v>
       </c>
@@ -6125,7 +6110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>276</v>
       </c>
@@ -6160,7 +6145,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>277</v>
       </c>
@@ -6195,7 +6180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>272</v>
       </c>
@@ -6230,7 +6215,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>273</v>
       </c>
@@ -6265,7 +6250,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>274</v>
       </c>
@@ -6300,7 +6285,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>270</v>
       </c>
@@ -6335,7 +6320,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>271</v>
       </c>
@@ -6370,7 +6355,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>283</v>
       </c>
@@ -6405,7 +6390,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>280</v>
       </c>
@@ -6440,7 +6425,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>281</v>
       </c>
@@ -6475,7 +6460,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>282</v>
       </c>
@@ -6510,7 +6495,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>278</v>
       </c>
@@ -6545,7 +6530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>279</v>
       </c>
@@ -6580,7 +6565,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>286</v>
       </c>
@@ -6615,7 +6600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>287</v>
       </c>
@@ -6650,7 +6635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>288</v>
       </c>
@@ -6685,7 +6670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>285</v>
       </c>
@@ -6720,7 +6705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>284</v>
       </c>
@@ -6755,7 +6740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>294</v>
       </c>
@@ -6790,7 +6775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>295</v>
       </c>
@@ -6825,7 +6810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>291</v>
       </c>
@@ -6860,7 +6845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>292</v>
       </c>
@@ -6895,7 +6880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>293</v>
       </c>
@@ -6930,7 +6915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>289</v>
       </c>
@@ -6965,7 +6950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>290</v>
       </c>
@@ -7000,7 +6985,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>301</v>
       </c>
@@ -7035,7 +7020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>302</v>
       </c>
@@ -7070,7 +7055,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>298</v>
       </c>
@@ -7105,7 +7090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>299</v>
       </c>
@@ -7140,7 +7125,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>300</v>
       </c>
@@ -7175,7 +7160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>296</v>
       </c>
@@ -7210,7 +7195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>297</v>
       </c>
@@ -7245,7 +7230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>251</v>
       </c>
@@ -7280,7 +7265,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>252</v>
       </c>
@@ -7315,7 +7300,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>207</v>
       </c>
@@ -7350,7 +7335,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>208</v>
       </c>
@@ -7385,7 +7370,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>209</v>
       </c>
@@ -7420,7 +7405,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>210</v>
       </c>
@@ -7455,7 +7440,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>205</v>
       </c>
@@ -7490,7 +7475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>206</v>
       </c>
@@ -7525,7 +7510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>202</v>
       </c>
@@ -7560,7 +7545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>203</v>
       </c>
@@ -7595,7 +7580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>204</v>
       </c>
@@ -7630,7 +7615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>200</v>
       </c>
@@ -7665,7 +7650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>201</v>
       </c>
@@ -7700,7 +7685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>196</v>
       </c>
@@ -7735,7 +7720,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>197</v>
       </c>
@@ -7770,7 +7755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>198</v>
       </c>
@@ -7805,7 +7790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>199</v>
       </c>
@@ -7840,7 +7825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>194</v>
       </c>
@@ -7875,7 +7860,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>195</v>
       </c>
@@ -7910,7 +7895,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>221</v>
       </c>
@@ -7945,7 +7930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>222</v>
       </c>
@@ -7980,7 +7965,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>223</v>
       </c>
@@ -8015,7 +8000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>219</v>
       </c>
@@ -8050,7 +8035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>220</v>
       </c>
@@ -8085,7 +8070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>217</v>
       </c>
@@ -8120,7 +8105,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>218</v>
       </c>
@@ -8155,7 +8140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>215</v>
       </c>
@@ -8190,7 +8175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>216</v>
       </c>
@@ -8225,7 +8210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>211</v>
       </c>
@@ -8260,7 +8245,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>212</v>
       </c>
@@ -8295,7 +8280,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>213</v>
       </c>
@@ -8330,7 +8315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>214</v>
       </c>
@@ -8365,7 +8350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>229</v>
       </c>
@@ -8400,7 +8385,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>226</v>
       </c>
@@ -8435,7 +8420,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>227</v>
       </c>
@@ -8470,7 +8455,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>228</v>
       </c>
@@ -8505,7 +8490,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>224</v>
       </c>
@@ -8540,7 +8525,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>225</v>
       </c>
@@ -8575,7 +8560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>236</v>
       </c>
@@ -8610,7 +8595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>237</v>
       </c>
@@ -8645,7 +8630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>238</v>
       </c>
@@ -8680,7 +8665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>234</v>
       </c>
@@ -8715,7 +8700,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>235</v>
       </c>
@@ -8750,7 +8735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>233</v>
       </c>
@@ -8785,7 +8770,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>230</v>
       </c>
@@ -8820,7 +8805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>231</v>
       </c>
@@ -8855,7 +8840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>232</v>
       </c>
@@ -8890,7 +8875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>257</v>
       </c>
@@ -8925,7 +8910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>242</v>
       </c>
@@ -8960,7 +8945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>243</v>
       </c>
@@ -8995,7 +8980,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>244</v>
       </c>
@@ -9030,7 +9015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>240</v>
       </c>
@@ -9065,7 +9050,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>241</v>
       </c>
@@ -9100,7 +9085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>239</v>
       </c>
@@ -9135,7 +9120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>248</v>
       </c>
@@ -9170,7 +9155,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>249</v>
       </c>
@@ -9205,7 +9190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>250</v>
       </c>
@@ -9240,7 +9225,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>246</v>
       </c>
@@ -9275,7 +9260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>247</v>
       </c>
@@ -9310,7 +9295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>245</v>
       </c>
@@ -9345,7 +9330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>81</v>
       </c>
@@ -9380,7 +9365,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>453</v>
       </c>
@@ -9415,7 +9400,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>79</v>
       </c>
@@ -9450,7 +9435,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>119</v>
       </c>
@@ -9485,7 +9470,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>82</v>
       </c>
@@ -9520,7 +9505,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>85</v>
       </c>
@@ -9555,7 +9540,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>122</v>
       </c>
@@ -9590,7 +9575,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>75</v>
       </c>
@@ -9625,7 +9610,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>124</v>
       </c>
@@ -9660,7 +9645,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>72</v>
       </c>
@@ -9695,7 +9680,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>127</v>
       </c>
@@ -9730,7 +9715,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>487</v>
       </c>
@@ -9765,7 +9750,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>91</v>
       </c>
@@ -9800,7 +9785,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>463</v>
       </c>
@@ -9835,7 +9820,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>461</v>
       </c>
@@ -9870,7 +9855,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>438</v>
       </c>
@@ -9905,7 +9890,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>450</v>
       </c>
@@ -9940,7 +9925,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>97</v>
       </c>
@@ -9975,7 +9960,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>88</v>
       </c>
@@ -10010,7 +9995,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>149</v>
       </c>
@@ -10045,7 +10030,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>466</v>
       </c>
@@ -10080,7 +10065,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>132</v>
       </c>
@@ -10115,7 +10100,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>129</v>
       </c>
@@ -10150,7 +10135,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>68</v>
       </c>
@@ -10185,7 +10170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>64</v>
       </c>
@@ -10220,7 +10205,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>150</v>
       </c>
@@ -10255,7 +10240,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>153</v>
       </c>
@@ -10290,7 +10275,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>485</v>
       </c>
@@ -10325,7 +10310,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>488</v>
       </c>
@@ -10363,7 +10348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>491</v>
       </c>
@@ -10401,7 +10386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>493</v>
       </c>
@@ -10439,7 +10424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>495</v>
       </c>
@@ -10477,7 +10462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>497</v>
       </c>
@@ -10515,7 +10500,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>500</v>
       </c>
@@ -10553,7 +10538,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>502</v>
       </c>
@@ -10591,7 +10576,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>504</v>
       </c>
@@ -10629,7 +10614,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>506</v>
       </c>
@@ -10667,7 +10652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>509</v>
       </c>
@@ -10705,7 +10690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>511</v>
       </c>
@@ -10743,7 +10728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>513</v>
       </c>
@@ -10781,7 +10766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>515</v>
       </c>
@@ -10819,7 +10804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>518</v>
       </c>
@@ -10857,7 +10842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>520</v>
       </c>
@@ -10895,7 +10880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>522</v>
       </c>
@@ -10933,7 +10918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>524</v>
       </c>
@@ -10971,7 +10956,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>527</v>
       </c>
@@ -11009,7 +10994,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>529</v>
       </c>
@@ -11047,7 +11032,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>531</v>
       </c>
@@ -11085,7 +11070,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>533</v>
       </c>
@@ -11123,7 +11108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>534</v>
       </c>
@@ -11161,7 +11146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>535</v>
       </c>
@@ -11199,7 +11184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>536</v>
       </c>
@@ -11237,7 +11222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>537</v>
       </c>
@@ -11275,7 +11260,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>539</v>
       </c>
@@ -11313,7 +11298,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>540</v>
       </c>
@@ -11351,7 +11336,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>542</v>
       </c>
@@ -11389,7 +11374,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>543</v>
       </c>
@@ -11427,7 +11412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>545</v>
       </c>
@@ -11465,7 +11450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>546</v>
       </c>
@@ -11503,7 +11488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>547</v>
       </c>
@@ -11541,7 +11526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>548</v>
       </c>
@@ -11579,7 +11564,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>550</v>
       </c>
@@ -11617,7 +11602,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>551</v>
       </c>
@@ -11655,7 +11640,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>552</v>
       </c>
@@ -11693,7 +11678,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>553</v>
       </c>
@@ -11731,7 +11716,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>554</v>
       </c>
@@ -11769,7 +11754,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>555</v>
       </c>
@@ -11807,7 +11792,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>556</v>
       </c>
@@ -11845,7 +11830,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>558</v>
       </c>
@@ -11883,7 +11868,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>559</v>
       </c>
@@ -11921,7 +11906,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>560</v>
       </c>
@@ -11959,7 +11944,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>561</v>
       </c>
@@ -11997,7 +11982,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>563</v>
       </c>
@@ -12035,7 +12020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>564</v>
       </c>
@@ -12073,7 +12058,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>565</v>
       </c>
@@ -12111,7 +12096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>566</v>
       </c>
@@ -12149,7 +12134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>572</v>
       </c>
@@ -12187,7 +12172,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>573</v>
       </c>
@@ -12225,7 +12210,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>574</v>
       </c>
@@ -12263,7 +12248,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>575</v>
       </c>
@@ -12301,7 +12286,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>577</v>
       </c>
@@ -12339,7 +12324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>578</v>
       </c>
@@ -12377,7 +12362,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>579</v>
       </c>
@@ -12415,7 +12400,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>580</v>
       </c>
@@ -12453,7 +12438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>582</v>
       </c>
@@ -12491,7 +12476,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>583</v>
       </c>
@@ -12529,7 +12514,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>584</v>
       </c>
@@ -12567,7 +12552,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>585</v>
       </c>
@@ -12605,7 +12590,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>587</v>
       </c>
@@ -12643,7 +12628,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>588</v>
       </c>
@@ -12681,7 +12666,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>589</v>
       </c>
@@ -12719,7 +12704,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>590</v>
       </c>
@@ -12757,7 +12742,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>592</v>
       </c>
@@ -12795,7 +12780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>593</v>
       </c>
@@ -12833,7 +12818,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>594</v>
       </c>
@@ -12871,7 +12856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>595</v>
       </c>
@@ -12909,7 +12894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>597</v>
       </c>
@@ -12947,7 +12932,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>598</v>
       </c>
@@ -12985,7 +12970,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>599</v>
       </c>
@@ -13023,7 +13008,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>600</v>
       </c>
@@ -13061,7 +13046,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>602</v>
       </c>
@@ -13099,7 +13084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>603</v>
       </c>
@@ -13137,7 +13122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="273" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>604</v>
       </c>
@@ -13175,7 +13160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="274" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>605</v>
       </c>
@@ -13213,7 +13198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="275" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>607</v>
       </c>
@@ -13251,7 +13236,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="276" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>608</v>
       </c>
@@ -13289,7 +13274,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="277" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>609</v>
       </c>
@@ -13327,7 +13312,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="278" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>610</v>
       </c>
@@ -13365,7 +13350,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="279" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>612</v>
       </c>
@@ -13403,7 +13388,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="280" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>613</v>
       </c>
@@ -13441,7 +13426,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="281" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>614</v>
       </c>
@@ -13479,7 +13464,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="282" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>615</v>
       </c>
@@ -13517,7 +13502,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="283" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>617</v>
       </c>
@@ -13555,7 +13540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="284" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>618</v>
       </c>
@@ -13593,7 +13578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="285" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>619</v>
       </c>
@@ -13631,7 +13616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>620</v>
       </c>
@@ -13669,7 +13654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>622</v>
       </c>
@@ -13707,7 +13692,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>623</v>
       </c>
@@ -13745,7 +13730,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>624</v>
       </c>
@@ -13783,7 +13768,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>625</v>
       </c>
@@ -13821,7 +13806,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>627</v>
       </c>
@@ -13859,7 +13844,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>628</v>
       </c>
@@ -13897,7 +13882,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>629</v>
       </c>
@@ -13935,7 +13920,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>630</v>
       </c>
@@ -13973,7 +13958,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>632</v>
       </c>
@@ -14011,7 +13996,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>633</v>
       </c>
@@ -14049,7 +14034,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>634</v>
       </c>
@@ -14087,7 +14072,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>635</v>
       </c>
@@ -14125,7 +14110,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>637</v>
       </c>
@@ -14163,7 +14148,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>638</v>
       </c>
@@ -14201,7 +14186,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>639</v>
       </c>
@@ -14239,7 +14224,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>640</v>
       </c>
@@ -14277,7 +14262,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>642</v>
       </c>
@@ -14315,7 +14300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>643</v>
       </c>
@@ -14353,7 +14338,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>644</v>
       </c>
@@ -14391,7 +14376,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="306" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>645</v>
       </c>
@@ -14429,7 +14414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="307" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>647</v>
       </c>
@@ -14467,7 +14452,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="308" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>648</v>
       </c>
@@ -14505,7 +14490,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="309" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>649</v>
       </c>
@@ -14543,7 +14528,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="310" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>650</v>
       </c>
@@ -14581,7 +14566,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="311" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>652</v>
       </c>
@@ -14619,7 +14604,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="312" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>653</v>
       </c>
@@ -14657,7 +14642,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="313" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>654</v>
       </c>
@@ -14695,7 +14680,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="314" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>655</v>
       </c>
@@ -14733,7 +14718,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>657</v>
       </c>
@@ -14771,7 +14756,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="316" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>658</v>
       </c>
@@ -14809,7 +14794,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="317" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>659</v>
       </c>
@@ -14847,7 +14832,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="318" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>660</v>
       </c>
@@ -14885,7 +14870,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="319" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>662</v>
       </c>
@@ -14923,7 +14908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="320" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>663</v>
       </c>
@@ -14961,7 +14946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="321" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>664</v>
       </c>
@@ -14999,7 +14984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="322" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>665</v>
       </c>
@@ -15037,7 +15022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="323" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>671</v>
       </c>
@@ -15075,7 +15060,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="324" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>672</v>
       </c>
@@ -15113,7 +15098,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="325" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>673</v>
       </c>
@@ -15151,7 +15136,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="326" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>674</v>
       </c>
@@ -15189,7 +15174,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="327" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>676</v>
       </c>
@@ -15227,7 +15212,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="328" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>677</v>
       </c>
@@ -15265,7 +15250,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="329" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>678</v>
       </c>
@@ -15303,7 +15288,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="330" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>679</v>
       </c>
@@ -15341,7 +15326,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="331" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>681</v>
       </c>
@@ -15379,7 +15364,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="332" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>682</v>
       </c>
@@ -15417,7 +15402,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="333" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>683</v>
       </c>
@@ -15455,7 +15440,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="334" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>684</v>
       </c>
@@ -15493,7 +15478,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="335" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>686</v>
       </c>
@@ -15531,7 +15516,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="336" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>687</v>
       </c>
@@ -15569,7 +15554,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="337" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>688</v>
       </c>
@@ -15607,7 +15592,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="338" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>689</v>
       </c>
@@ -15645,7 +15630,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="339" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>691</v>
       </c>
@@ -15683,7 +15668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="340" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>692</v>
       </c>
@@ -15721,7 +15706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="341" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>693</v>
       </c>
@@ -15759,7 +15744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="342" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>694</v>
       </c>
@@ -15797,7 +15782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="343" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>696</v>
       </c>
@@ -15835,7 +15820,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="344" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>697</v>
       </c>
@@ -15873,7 +15858,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="345" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>698</v>
       </c>
@@ -15911,7 +15896,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="346" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>699</v>
       </c>
@@ -15949,7 +15934,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="347" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>701</v>
       </c>
@@ -15987,7 +15972,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="348" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>702</v>
       </c>
@@ -16025,7 +16010,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="349" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>703</v>
       </c>
@@ -16063,7 +16048,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="350" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>704</v>
       </c>
@@ -16101,7 +16086,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="351" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>706</v>
       </c>
@@ -16139,7 +16124,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="352" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>707</v>
       </c>
@@ -16177,7 +16162,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="353" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>708</v>
       </c>
@@ -16215,7 +16200,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="354" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>709</v>
       </c>
@@ -16253,7 +16238,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="355" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>711</v>
       </c>
@@ -16291,7 +16276,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="356" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>712</v>
       </c>
@@ -16329,7 +16314,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="357" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>713</v>
       </c>
@@ -16367,7 +16352,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="358" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>714</v>
       </c>
@@ -16405,7 +16390,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="359" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>716</v>
       </c>
@@ -16443,7 +16428,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="360" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>717</v>
       </c>
@@ -16481,7 +16466,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="361" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>718</v>
       </c>
@@ -16519,7 +16504,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="362" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>719</v>
       </c>
@@ -16557,7 +16542,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="363" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>720</v>
       </c>
@@ -16595,7 +16580,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="364" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>721</v>
       </c>
@@ -16633,7 +16618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="365" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>722</v>
       </c>
@@ -16671,7 +16656,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="366" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>723</v>
       </c>
@@ -16709,7 +16694,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="367" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>724</v>
       </c>
@@ -16747,7 +16732,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="368" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>725</v>
       </c>
@@ -16785,7 +16770,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="369" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
         <v>726</v>
       </c>
@@ -16823,7 +16808,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="370" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
         <v>727</v>
       </c>
@@ -16861,7 +16846,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="371" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
         <v>728</v>
       </c>
@@ -16899,7 +16884,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="372" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
         <v>729</v>
       </c>
@@ -16937,7 +16922,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="373" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
         <v>730</v>
       </c>
@@ -16975,7 +16960,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="374" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
         <v>731</v>
       </c>
@@ -17013,7 +16998,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="375" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
         <v>732</v>
       </c>
@@ -17051,7 +17036,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="376" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
         <v>733</v>
       </c>
@@ -17089,7 +17074,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="377" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
         <v>734</v>
       </c>
@@ -17127,7 +17112,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="378" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
         <v>735</v>
       </c>
@@ -17165,7 +17150,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="379" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
         <v>761</v>
       </c>
@@ -17200,7 +17185,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="380" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
         <v>762</v>
       </c>
@@ -17235,7 +17220,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="381" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
         <v>763</v>
       </c>
@@ -17270,7 +17255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="382" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
         <v>764</v>
       </c>
@@ -17305,7 +17290,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="383" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
         <v>765</v>
       </c>
@@ -17340,7 +17325,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="384" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
         <v>766</v>
       </c>
@@ -17375,7 +17360,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="385" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
         <v>767</v>
       </c>
@@ -17410,7 +17395,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="386" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
         <v>768</v>
       </c>
@@ -17445,7 +17430,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="387" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
         <v>769</v>
       </c>
@@ -17480,7 +17465,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="388" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
         <v>770</v>
       </c>
@@ -17515,7 +17500,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
         <v>771</v>
       </c>
@@ -17550,7 +17535,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="390" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
         <v>772</v>
       </c>
@@ -17585,7 +17570,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="391" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
         <v>773</v>
       </c>
@@ -17620,7 +17605,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="392" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
         <v>774</v>
       </c>
@@ -17655,7 +17640,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="393" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
         <v>775</v>
       </c>
@@ -17690,7 +17675,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="394" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
         <v>776</v>
       </c>
@@ -17725,7 +17710,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="395" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
         <v>777</v>
       </c>
@@ -17760,7 +17745,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="396" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
         <v>778</v>
       </c>
@@ -17795,7 +17780,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="397" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
         <v>779</v>
       </c>
@@ -17830,7 +17815,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="398" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
         <v>810</v>
       </c>
@@ -17865,7 +17850,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
         <v>811</v>
       </c>
@@ -17900,7 +17885,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="400" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
         <v>812</v>
       </c>
@@ -17935,7 +17920,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="401" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
         <v>813</v>
       </c>
@@ -17970,7 +17955,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="402" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
         <v>814</v>
       </c>
@@ -18005,7 +17990,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="403" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
         <v>825</v>
       </c>
@@ -18040,7 +18025,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="404" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
         <v>826</v>
       </c>
@@ -18075,7 +18060,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="405" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
         <v>827</v>
       </c>
@@ -18110,7 +18095,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="406" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
         <v>828</v>
       </c>
@@ -18145,7 +18130,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="407" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
         <v>829</v>
       </c>
@@ -18180,7 +18165,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="408" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
         <v>830</v>
       </c>
@@ -18215,7 +18200,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="409" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
         <v>831</v>
       </c>
@@ -18250,7 +18235,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="410" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
         <v>832</v>
       </c>
@@ -18285,7 +18270,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="411" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
         <v>833</v>
       </c>
@@ -18320,7 +18305,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="412" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
         <v>834</v>
       </c>
@@ -18355,7 +18340,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="413" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
         <v>835</v>
       </c>
@@ -18390,7 +18375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="414" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
         <v>836</v>
       </c>
@@ -18425,7 +18410,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="415" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
         <v>837</v>
       </c>
@@ -18460,7 +18445,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="416" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
         <v>838</v>
       </c>
@@ -18495,7 +18480,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="417" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
         <v>839</v>
       </c>
@@ -18530,7 +18515,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="418" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
         <v>840</v>
       </c>
@@ -18565,7 +18550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="419" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
         <v>841</v>
       </c>
@@ -18600,7 +18585,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="420" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
         <v>842</v>
       </c>
@@ -18635,7 +18620,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="421" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
         <v>843</v>
       </c>
@@ -18670,7 +18655,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="422" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
         <v>881</v>
       </c>
@@ -18705,7 +18690,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="423" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
         <v>882</v>
       </c>
@@ -18740,7 +18725,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="424" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
         <v>887</v>
       </c>
@@ -18775,7 +18760,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="425" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
         <v>888</v>
       </c>
@@ -18810,7 +18795,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="426" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
         <v>892</v>
       </c>
@@ -18845,7 +18830,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="427" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
         <v>895</v>
       </c>
@@ -18880,7 +18865,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="428" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
         <v>897</v>
       </c>
@@ -19246,7 +19231,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19307,8 +19292,8 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>303</v>
+      <c r="A2" s="4" t="s">
+        <v>572</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>162</v>
@@ -19323,7 +19308,7 @@
       </c>
       <c r="E2" s="2">
         <f>_xlfn.XLOOKUP(A2,CATALOGO_PRODUCTOS!A:A,CATALOGO_PRODUCTOS!B:B,0,0)</f>
-        <v>2.35E-2</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2">
         <f>_xlfn.XLOOKUP(D2,TIPOS_CAMBIO!A:A,TIPOS_CAMBIO!B:B,"",0)</f>
@@ -19331,7 +19316,7 @@
       </c>
       <c r="G2" s="7">
         <f>$E2*$F2</f>
-        <v>0.49349999999999999</v>
+        <v>273</v>
       </c>
       <c r="H2" s="8">
         <f>_xlfn.XLOOKUP($B$2,PARAMETROS_IMPORTACION!A:A,PARAMETROS_IMPORTACION!C:C,0,0)</f>
@@ -19359,11 +19344,11 @@
       </c>
       <c r="N2" s="2">
         <f>IF($C2="Importado",$G2*(1+$H2+I2+$J2+$L2+$M2),$G2)</f>
-        <v>0.55197974999999999</v>
+        <v>305.35050000000001</v>
       </c>
       <c r="O2" s="2">
         <f>N2 * (1 + K2)</f>
-        <v>0.607177725</v>
+        <v>335.88555000000002</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>